<commit_message>
Edit test progran check to xml & excel
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90983009-A44F-4F4B-A1A6-50226E09A27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309ACDA0-A6AD-4336-8E21-2D8EC5CB3DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>9E82889C248D6BEF848E1AFB27808B21</t>
+  </si>
+  <si>
+    <t>بررسی برنامه تست</t>
   </si>
 </sst>
 </file>
@@ -283,6 +286,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -299,9 +305,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,7 +591,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,41 +627,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:94" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="16"/>
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
@@ -671,7 +674,9 @@
       <c r="E2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
@@ -740,7 +745,7 @@
       </c>
     </row>
     <row r="3" spans="1:94" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -4681,7 +4686,7 @@
     </row>
     <row r="153" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
-      <c r="B153" s="16"/>
+      <c r="B153" s="10"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
@@ -4708,7 +4713,7 @@
     </row>
     <row r="154" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
-      <c r="B154" s="16"/>
+      <c r="B154" s="10"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
@@ -4734,7 +4739,7 @@
     </row>
     <row r="155" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
-      <c r="B155" s="16"/>
+      <c r="B155" s="10"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
@@ -4760,7 +4765,7 @@
     </row>
     <row r="156" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
-      <c r="B156" s="16"/>
+      <c r="B156" s="10"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
@@ -4787,7 +4792,7 @@
     </row>
     <row r="157" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
-      <c r="B157" s="16"/>
+      <c r="B157" s="10"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
@@ -4813,7 +4818,7 @@
     </row>
     <row r="158" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A158" s="7"/>
-      <c r="B158" s="16"/>
+      <c r="B158" s="10"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
@@ -4839,7 +4844,7 @@
     </row>
     <row r="159" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A159" s="7"/>
-      <c r="B159" s="16"/>
+      <c r="B159" s="10"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
@@ -4865,7 +4870,7 @@
     </row>
     <row r="160" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
-      <c r="B160" s="16"/>
+      <c r="B160" s="10"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
@@ -4891,7 +4896,7 @@
     </row>
     <row r="161" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
-      <c r="B161" s="16"/>
+      <c r="B161" s="10"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
@@ -4917,7 +4922,7 @@
     </row>
     <row r="162" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
-      <c r="B162" s="16"/>
+      <c r="B162" s="10"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
@@ -18473,20 +18478,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B153:B162"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="V2:V3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="U2:U3"/>
@@ -18503,6 +18494,20 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="B1:AB1"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B153:B162"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="V2:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit test modem to xml & excel
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E9B259-13E5-4D37-ADC5-B62BC7F8D963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765AF59B-9C47-4ED0-B5DF-53C10231F301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -600,7 +600,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,8 @@
     <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="19.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" style="1" customWidth="1"/>
     <col min="12" max="13" width="9.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
@@ -695,7 +696,9 @@
       <c r="G2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="I2" s="10"/>
       <c r="J2" s="8"/>
       <c r="K2" s="10" t="s">

</xml_diff>

<commit_message>
Edit test voltage rtc to xml & excel
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765AF59B-9C47-4ED0-B5DF-53C10231F301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568764A2-F024-44D6-81EA-B0127FEC10AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">اتصال تغذیه 4 ولت </t>
+  </si>
+  <si>
+    <t>بررسی ولتاژ باتری ساعت</t>
   </si>
 </sst>
 </file>
@@ -599,8 +602,8 @@
   <dimension ref="A1:CT1504"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I9" sqref="I9"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +616,8 @@
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" style="1" customWidth="1"/>
     <col min="12" max="13" width="9.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
@@ -699,7 +703,9 @@
       <c r="H2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="J2" s="8"/>
       <c r="K2" s="10" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Add eeprom check to excel
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C25541-D9A1-4336-A14B-8588A30D91B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3123FA68-FEC7-4A15-B722-67118D7B9C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>بررسی ولتاژ باتری ساعت</t>
+  </si>
+  <si>
+    <t>عملکرد ایپرام خارجی</t>
   </si>
 </sst>
 </file>
@@ -298,9 +301,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -317,6 +317,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L7" sqref="L7"/>
+      <selection pane="topRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,48 +646,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:101" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="18"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="17"/>
     </row>
     <row r="2" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
@@ -712,7 +715,9 @@
       <c r="J2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="8"/>
+      <c r="K2" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="10" t="s">
@@ -780,7 +785,7 @@
       </c>
     </row>
     <row r="3" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -790,7 +795,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="9"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="11"/>
@@ -5770,7 +5775,7 @@
     </row>
     <row r="153" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
-      <c r="B153" s="12"/>
+      <c r="B153" s="18"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
@@ -5804,7 +5809,7 @@
     </row>
     <row r="154" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
-      <c r="B154" s="12"/>
+      <c r="B154" s="18"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
@@ -5837,7 +5842,7 @@
     </row>
     <row r="155" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
-      <c r="B155" s="12"/>
+      <c r="B155" s="18"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
@@ -5870,7 +5875,7 @@
     </row>
     <row r="156" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
-      <c r="B156" s="12"/>
+      <c r="B156" s="18"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
@@ -5904,7 +5909,7 @@
     </row>
     <row r="157" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
-      <c r="B157" s="12"/>
+      <c r="B157" s="18"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
@@ -5937,7 +5942,7 @@
     </row>
     <row r="158" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A158" s="7"/>
-      <c r="B158" s="12"/>
+      <c r="B158" s="18"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
@@ -5970,7 +5975,7 @@
     </row>
     <row r="159" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A159" s="7"/>
-      <c r="B159" s="12"/>
+      <c r="B159" s="18"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
@@ -6003,7 +6008,7 @@
     </row>
     <row r="160" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
-      <c r="B160" s="12"/>
+      <c r="B160" s="18"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
@@ -6036,7 +6041,7 @@
     </row>
     <row r="161" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
-      <c r="B161" s="12"/>
+      <c r="B161" s="18"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
@@ -6069,7 +6074,7 @@
     </row>
     <row r="162" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
-      <c r="B162" s="12"/>
+      <c r="B162" s="18"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
@@ -22760,7 +22765,25 @@
       <c r="A1504" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="B153:B162"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="B1:AI1"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="U2:U3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="A1:A3"/>
@@ -22777,23 +22800,6 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B1:AI1"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="B153:B162"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add lcd check to excel
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA19C123-0C67-401D-A938-1F11D21ADA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480070C-FA3F-43E5-A5BB-D3C5879E7BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>عملکرد ایپرام خارجی</t>
+  </si>
+  <si>
+    <t>عملکرد نمایشگر</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <selection pane="topRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +623,9 @@
     <col min="7" max="7" width="17.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" style="1" customWidth="1"/>
-    <col min="10" max="13" width="17.42578125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="17.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" style="1" customWidth="1"/>
     <col min="15" max="16" width="9.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="1" customWidth="1"/>
@@ -718,7 +723,9 @@
       <c r="K2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="M2" s="8"/>
       <c r="N2" s="10" t="s">
         <v>13</v>
@@ -796,7 +803,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="9"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="9"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -22765,7 +22772,7 @@
       <c r="A1504" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
     <mergeCell ref="B153:B162"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="O2:O3"/>
@@ -22779,6 +22786,7 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
     <mergeCell ref="B1:AI1"/>
     <mergeCell ref="AH2:AH3"/>
     <mergeCell ref="Y2:Y3"/>

</xml_diff>

<commit_message>
Add test buzzer to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041B19E4-08E3-4529-88F8-55F7FE355105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80595CA3-D291-491E-AEEF-19F4ED5C306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>عملکرد OP</t>
+  </si>
+  <si>
+    <t>عملکرد Buzzer</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L11" sqref="L11"/>
+      <selection pane="topRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +737,9 @@
       <c r="L2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="11"/>
+      <c r="M2" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>

</xml_diff>

<commit_message>
Add test led red to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80595CA3-D291-491E-AEEF-19F4ED5C306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8565FE3-D62F-4846-A796-7E45EAA22419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>عملکرد Buzzer</t>
+  </si>
+  <si>
+    <t>عملکرد ال ای دی Red</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L10" sqref="L10"/>
+      <selection pane="topRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +743,9 @@
       <c r="M2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="11"/>
+      <c r="N2" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11" t="s">

</xml_diff>

<commit_message>
Add test tamper switch to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8565FE3-D62F-4846-A796-7E45EAA22419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86036D88-489E-4484-A055-1A294FAB5A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>عملکرد ال ای دی Red</t>
+  </si>
+  <si>
+    <t>عملکرد کلید Tamper</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N9" sqref="N9"/>
+      <selection pane="topRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +749,9 @@
       <c r="N2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="11"/>
+      <c r="O2" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Add test lcd switch to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86036D88-489E-4484-A055-1A294FAB5A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB9B9CE-3358-4FA0-8B45-4BAAE90CF27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -620,8 +620,8 @@
   <dimension ref="A1:DB923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O7" sqref="O7"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
     <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" style="1" customWidth="1"/>
     <col min="10" max="16" width="17.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.42578125" style="1" customWidth="1"/>
     <col min="19" max="19" width="9.85546875" style="1" customWidth="1"/>
     <col min="20" max="21" width="9.28515625" style="1" customWidth="1"/>
@@ -752,10 +752,10 @@
       <c r="O2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11" t="s">
         <v>13</v>
@@ -899,9 +899,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>

</xml_diff>

<commit_message>
Add test reset parm to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB9B9CE-3358-4FA0-8B45-4BAAE90CF27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7586ACF3-A477-44B7-9AE4-2266B130539C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>عملکرد کلید Tamper</t>
+  </si>
+  <si>
+    <t>ریست نمودن پارامتر ها</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q4" sqref="Q4"/>
+      <selection pane="topRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +758,9 @@
       <c r="P2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="11"/>
+      <c r="Q2" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="R2" s="11"/>
       <c r="S2" s="11" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Add test clear sql to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7586ACF3-A477-44B7-9AE4-2266B130539C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833CD1F8-B3AA-4B72-9C40-336515B364DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>ریست نمودن پارامتر ها</t>
+  </si>
+  <si>
+    <t>پاک نمودن پایگاه داده</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="topRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +764,9 @@
       <c r="Q2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="11"/>
+      <c r="R2" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="S2" s="11" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add test set datetime to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E75D74-A2E9-4245-89A5-CC5253297A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A836C6-4144-4263-8195-190E14EC27C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>تنظیم سریال</t>
+  </si>
+  <si>
+    <t>تنظیم ساعت و تاریخ</t>
   </si>
 </sst>
 </file>
@@ -630,7 +633,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S4" sqref="S4"/>
+      <selection pane="topRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +779,9 @@
       <c r="S2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="11"/>
+      <c r="T2" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="U2" s="11"/>
       <c r="V2" s="11" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Add test voltage power to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FEC5E2-0760-455F-9F8C-3BE8BC58447A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976AFD46-D424-4D8F-85B5-A6B0BB9F5EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -110,6 +110,21 @@
   </si>
   <si>
     <t>راه اندازی برنامه نهایی</t>
+  </si>
+  <si>
+    <t>بررسی تغذیه 12 ولت</t>
+  </si>
+  <si>
+    <t>بررسی تغذیه 5 ولت</t>
+  </si>
+  <si>
+    <t>بررسی تغذیه 4 ولت</t>
+  </si>
+  <si>
+    <t>بررسی تغذیه 3.3 ولت</t>
+  </si>
+  <si>
+    <t>بررسی Booster</t>
   </si>
 </sst>
 </file>
@@ -584,8 +599,8 @@
   <dimension ref="A1:CY923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V7" sqref="V7"/>
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,11 +741,21 @@
       <c r="U2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
+      <c r="V2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="AA2" s="11"/>
       <c r="AB2" s="11"/>
       <c r="AC2" s="11"/>

</xml_diff>

<commit_message>
Add test relay power to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976AFD46-D424-4D8F-85B5-A6B0BB9F5EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507A5820-B10A-4D9B-AB61-EDC174ADBAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>بررسی Booster</t>
+  </si>
+  <si>
+    <t>بررسی عملکرد رله</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z7" sqref="Z7"/>
+      <selection pane="topRight" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +625,7 @@
     <col min="24" max="24" width="19.140625" style="1" customWidth="1"/>
     <col min="25" max="25" width="20.42578125" style="1" customWidth="1"/>
     <col min="26" max="26" width="18.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" style="1" customWidth="1"/>
     <col min="28" max="28" width="13" style="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="1" customWidth="1"/>
     <col min="30" max="30" width="12.42578125" style="1" customWidth="1"/>
@@ -756,7 +759,9 @@
       <c r="Z2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="11"/>
+      <c r="AA2" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="AB2" s="11"/>
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>

</xml_diff>

<commit_message>
Add test RS485 power to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507A5820-B10A-4D9B-AB61-EDC174ADBAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB47A2A-1B38-46C6-B3A8-08241904825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>بررسی عملکرد رله</t>
+  </si>
+  <si>
+    <t>بررسی عملکرد RS485</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA6" sqref="AA6"/>
+      <selection pane="topRight" activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +629,7 @@
     <col min="25" max="25" width="20.42578125" style="1" customWidth="1"/>
     <col min="26" max="26" width="18.140625" style="1" customWidth="1"/>
     <col min="27" max="27" width="14.5703125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13" style="1" customWidth="1"/>
+    <col min="28" max="28" width="17.28515625" style="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="1" customWidth="1"/>
     <col min="30" max="30" width="12.42578125" style="1" customWidth="1"/>
     <col min="31" max="31" width="15.140625" style="1" customWidth="1"/>
@@ -762,7 +765,9 @@
       <c r="AA2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="11"/>
+      <c r="AB2" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
       <c r="AE2" s="11"/>

</xml_diff>

<commit_message>
Add test MBUS power to excel file
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB47A2A-1B38-46C6-B3A8-08241904825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF233FD4-BC1B-43A1-ACF1-06FC10E6C066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>بررسی عملکرد RS485</t>
+  </si>
+  <si>
+    <t>بررسی عملکرد MBUS</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB8" sqref="AB8"/>
+      <selection pane="topRight" activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +633,7 @@
     <col min="26" max="26" width="18.140625" style="1" customWidth="1"/>
     <col min="27" max="27" width="14.5703125" style="1" customWidth="1"/>
     <col min="28" max="28" width="17.28515625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11" style="1" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="1" customWidth="1"/>
     <col min="30" max="30" width="12.42578125" style="1" customWidth="1"/>
     <col min="31" max="31" width="15.140625" style="1" customWidth="1"/>
     <col min="32" max="32" width="12.7109375" style="1" customWidth="1"/>
@@ -768,7 +771,9 @@
       <c r="AB2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="11"/>
+      <c r="AC2" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="AD2" s="11"/>
       <c r="AE2" s="11"/>
       <c r="AF2" s="11"/>

</xml_diff>

<commit_message>
Edit xml to check sum excel field
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7397D8-3671-4566-B73A-AB7A8C17E419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD470F93-6000-4935-83FA-3DCED21417C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>9E82889C248D6BEF848E1AFB27808B21</t>
   </si>
   <si>
     <t>بررسی برنامه تست</t>
@@ -136,10 +133,7 @@
     <t>بررسی عملکرد MBUS</t>
   </si>
   <si>
-    <t>تگ شروع از سیستم دریافت نگردید</t>
-  </si>
-  <si>
-    <t>253FA34D2090A212C17EE2B01A06C139</t>
+    <t>3CEEA4D328CB7107F29A5C53F0538283</t>
   </si>
 </sst>
 </file>
@@ -304,13 +298,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -614,8 +608,8 @@
   <dimension ref="A1:CU923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE8" sqref="AE8"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,141 +682,141 @@
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
+      <c r="J2" s="9" t="s">
+        <v>9</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>9</v>
+      <c r="L2" s="9" t="s">
+        <v>20</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="M2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="Q2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="W2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Y2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AA2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AB2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AC2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AE2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AG2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
     </row>
     <row r="4" spans="1:99" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -865,27 +859,33 @@
       <c r="V4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3">
-        <v>91900</v>
+      <c r="W4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="AG4" s="4" t="s">
         <v>11</v>
@@ -5348,7 +5348,7 @@
       <c r="AC152" s="3"/>
     </row>
     <row r="153" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B153" s="10"/>
+      <c r="B153" s="8"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
@@ -5379,7 +5379,7 @@
       <c r="AF153" s="6"/>
     </row>
     <row r="154" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B154" s="10"/>
+      <c r="B154" s="8"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
@@ -5409,7 +5409,7 @@
       <c r="AC154" s="3"/>
     </row>
     <row r="155" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B155" s="10"/>
+      <c r="B155" s="8"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
@@ -5439,7 +5439,7 @@
       <c r="AC155" s="3"/>
     </row>
     <row r="156" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B156" s="10"/>
+      <c r="B156" s="8"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
@@ -5470,7 +5470,7 @@
       <c r="AF156" s="6"/>
     </row>
     <row r="157" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B157" s="10"/>
+      <c r="B157" s="8"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
@@ -5500,7 +5500,7 @@
       <c r="AC157" s="3"/>
     </row>
     <row r="158" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B158" s="10"/>
+      <c r="B158" s="8"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
@@ -5530,7 +5530,7 @@
       <c r="AC158" s="3"/>
     </row>
     <row r="159" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B159" s="10"/>
+      <c r="B159" s="8"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
@@ -5560,7 +5560,7 @@
       <c r="AC159" s="3"/>
     </row>
     <row r="160" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B160" s="10"/>
+      <c r="B160" s="8"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
@@ -5590,7 +5590,7 @@
       <c r="AC160" s="3"/>
     </row>
     <row r="161" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B161" s="10"/>
+      <c r="B161" s="8"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
@@ -5620,7 +5620,7 @@
       <c r="AC161" s="3"/>
     </row>
     <row r="162" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B162" s="10"/>
+      <c r="B162" s="8"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
@@ -19019,6 +19019,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="V2:V3"/>
@@ -19030,6 +19036,8 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B1:AG1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AE2:AE3"/>
     <mergeCell ref="B153:B162"/>
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="W2:W3"/>
@@ -19042,18 +19050,10 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AG2:AG3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit led green and red for send and receive test
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD470F93-6000-4935-83FA-3DCED21417C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE9F4E3-96CD-44C0-AAC1-B1353B6EC154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5010" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestResult" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>سریال دستگاه ها</t>
   </si>
@@ -133,7 +133,10 @@
     <t>بررسی عملکرد MBUS</t>
   </si>
   <si>
-    <t>3CEEA4D328CB7107F29A5C53F0538283</t>
+    <t>C301B3C04089955B3B5AD891F6408100</t>
+  </si>
+  <si>
+    <t>1402-07-19 12:52:28</t>
   </si>
 </sst>
 </file>
@@ -298,9 +301,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -323,6 +323,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,177 +645,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="15"/>
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AA2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AC2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AD2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AE2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AF2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AG2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
     </row>
     <row r="4" spans="1:99" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -846,16 +849,36 @@
       <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="V4" s="3" t="s">
         <v>13</v>
       </c>
@@ -882,7 +905,7 @@
       </c>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3">
-        <v>1200</v>
+        <v>2800</v>
       </c>
       <c r="AF4" s="4" t="s">
         <v>37</v>
@@ -5348,7 +5371,7 @@
       <c r="AC152" s="3"/>
     </row>
     <row r="153" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B153" s="8"/>
+      <c r="B153" s="16"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
@@ -5379,7 +5402,7 @@
       <c r="AF153" s="6"/>
     </row>
     <row r="154" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B154" s="8"/>
+      <c r="B154" s="16"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
@@ -5409,7 +5432,7 @@
       <c r="AC154" s="3"/>
     </row>
     <row r="155" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B155" s="8"/>
+      <c r="B155" s="16"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
@@ -5439,7 +5462,7 @@
       <c r="AC155" s="3"/>
     </row>
     <row r="156" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B156" s="8"/>
+      <c r="B156" s="16"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
@@ -5470,7 +5493,7 @@
       <c r="AF156" s="6"/>
     </row>
     <row r="157" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B157" s="8"/>
+      <c r="B157" s="16"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
@@ -5500,7 +5523,7 @@
       <c r="AC157" s="3"/>
     </row>
     <row r="158" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B158" s="8"/>
+      <c r="B158" s="16"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
@@ -5530,7 +5553,7 @@
       <c r="AC158" s="3"/>
     </row>
     <row r="159" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B159" s="8"/>
+      <c r="B159" s="16"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
@@ -5560,7 +5583,7 @@
       <c r="AC159" s="3"/>
     </row>
     <row r="160" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B160" s="8"/>
+      <c r="B160" s="16"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
@@ -5590,7 +5613,7 @@
       <c r="AC160" s="3"/>
     </row>
     <row r="161" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B161" s="8"/>
+      <c r="B161" s="16"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
@@ -5620,7 +5643,7 @@
       <c r="AC161" s="3"/>
     </row>
     <row r="162" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B162" s="8"/>
+      <c r="B162" s="16"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
@@ -19019,9 +19042,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="AG2:AG3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="B153:B162"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="L2:L3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
@@ -19038,22 +19077,6 @@
     <mergeCell ref="B1:AG1"/>
     <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="B153:B162"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update xml file for version v90.14030202
</commit_message>
<xml_diff>
--- a/MWM/TestApp/_Files/Exel/MWM.xlsx
+++ b/MWM/TestApp/_Files/Exel/MWM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE9F4E3-96CD-44C0-AAC1-B1353B6EC154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DB454A-FA07-461C-AD0B-EC7F03C9CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestResult" sheetId="1" r:id="rId1"/>
@@ -133,10 +133,10 @@
     <t>بررسی عملکرد MBUS</t>
   </si>
   <si>
-    <t>C301B3C04089955B3B5AD891F6408100</t>
+    <t>1403-01-19 12:01:55</t>
   </si>
   <si>
-    <t>1402-07-19 12:52:28</t>
+    <t>C301B3C04089955B3B5AD891F6408100</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
         <v>13</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>13</v>
@@ -908,7 +908,7 @@
         <v>2800</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AG4" s="4" t="s">
         <v>11</v>
@@ -19042,11 +19042,12 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
     <mergeCell ref="AG2:AG3"/>
     <mergeCell ref="P2:P3"/>
+    <mergeCell ref="M2:M3"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="B153:B162"/>
     <mergeCell ref="Z2:Z3"/>
@@ -19060,10 +19061,9 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="V2:V3"/>

</xml_diff>